<commit_message>
This is the rendering of the sheet
</commit_message>
<xml_diff>
--- a/Sheets/July_Beverage_Inventory_2024_Luis.xlsx
+++ b/Sheets/July_Beverage_Inventory_2024_Luis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelangelweill/Documents/bootcamp/Hiyakawa-Inventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelangelweill/Documents/bootcamp/Hiyakawa-Inventory/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E435A40-B551-2248-A94A-D4EDD15569BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13D8D0-EC1C-364F-BB4F-632F89F65EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15260" windowHeight="16380" xr2:uid="{AA23DA77-A71A-4544-8D83-D05CD8F00C4B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AA23DA77-A71A-4544-8D83-D05CD8F00C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="July Inventory (2)" sheetId="1" r:id="rId1"/>
@@ -1159,7 +1159,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1190,6 +1193,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1337,8 +1346,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1363,10 +1373,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1387,11 +1393,16 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1405,10 +1416,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1733,9 +1740,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1745,8 +1752,8 @@
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="38.1640625" customWidth="1"/>
     <col min="5" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="15" style="30" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="15" style="26" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="33" customWidth="1"/>
     <col min="9" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1769,10 +1776,10 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="3"/>
@@ -1810,8 +1817,7 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -1845,8 +1851,10 @@
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="34">
+        <v>1</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1880,8 +1888,8 @@
       <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1915,8 +1923,8 @@
       <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1950,8 +1958,8 @@
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="34"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1987,8 +1995,8 @@
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -2022,8 +2030,8 @@
       <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -2057,8 +2065,8 @@
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -2092,8 +2100,8 @@
       <c r="F10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -2127,8 +2135,8 @@
       <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -2162,8 +2170,8 @@
       <c r="F12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -2197,8 +2205,8 @@
       <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -2232,8 +2240,8 @@
       <c r="F14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -2267,8 +2275,8 @@
       <c r="F15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -2302,8 +2310,8 @@
       <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -2337,8 +2345,8 @@
       <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2372,8 +2380,8 @@
       <c r="F18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2407,8 +2415,8 @@
       <c r="F19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2442,8 +2450,8 @@
       <c r="F20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2477,8 +2485,8 @@
       <c r="F21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2512,8 +2520,8 @@
       <c r="F22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2547,8 +2555,8 @@
       <c r="F23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2582,8 +2590,8 @@
       <c r="F24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2617,8 +2625,8 @@
       <c r="F25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2652,8 +2660,8 @@
       <c r="F26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="27"/>
-      <c r="H26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2687,8 +2695,8 @@
       <c r="F27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2722,8 +2730,8 @@
       <c r="F28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="34"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2757,8 +2765,8 @@
       <c r="F29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="34"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2792,8 +2800,8 @@
       <c r="F30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="34"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2827,8 +2835,8 @@
       <c r="F31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="34"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2862,8 +2870,8 @@
       <c r="F32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="27"/>
-      <c r="H32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="34"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2897,8 +2905,8 @@
       <c r="F33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="27"/>
-      <c r="H33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="34"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2932,8 +2940,8 @@
       <c r="F34" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="34"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2967,8 +2975,8 @@
       <c r="F35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="34"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -3002,8 +3010,8 @@
       <c r="F36" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G36" s="27"/>
-      <c r="H36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -3037,8 +3045,8 @@
       <c r="F37" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="27"/>
-      <c r="H37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="34"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -3072,8 +3080,8 @@
       <c r="F38" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="27"/>
-      <c r="H38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="34"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -3107,8 +3115,8 @@
       <c r="F39" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="34"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -3144,8 +3152,8 @@
       <c r="F40" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G40" s="27"/>
-      <c r="H40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="34"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -3162,42 +3170,42 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:23" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="31" t="s">
+    <row r="41" spans="1:23" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F41" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="G41" s="33"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="35"/>
-      <c r="V41" s="35"/>
-      <c r="W41" s="35"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="30"/>
+      <c r="V41" s="30"/>
+      <c r="W41" s="30"/>
     </row>
     <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
@@ -3218,8 +3226,8 @@
       <c r="F42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="27"/>
-      <c r="H42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="34"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -3253,10 +3261,10 @@
       <c r="F43" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="27" t="s">
+      <c r="G43" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="H43" s="23"/>
+      <c r="H43" s="34"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -3290,8 +3298,8 @@
       <c r="F44" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G44" s="27"/>
-      <c r="H44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="34"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -3325,8 +3333,8 @@
       <c r="F45" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="34"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -3360,8 +3368,8 @@
       <c r="F46" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="34"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -3395,8 +3403,8 @@
       <c r="F47" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="34"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -3430,8 +3438,8 @@
       <c r="F48" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G48" s="27"/>
-      <c r="H48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="34"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -3465,8 +3473,8 @@
       <c r="F49" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G49" s="27"/>
-      <c r="H49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="34"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -3500,8 +3508,8 @@
       <c r="F50" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="34"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -3535,8 +3543,8 @@
       <c r="F51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="27"/>
-      <c r="H51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="34"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -3572,8 +3580,8 @@
       <c r="F52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G52" s="27"/>
-      <c r="H52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="34"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -3609,8 +3617,8 @@
       <c r="F53" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G53" s="27"/>
-      <c r="H53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="34"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -3646,8 +3654,8 @@
       <c r="F54" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="34"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -3683,8 +3691,8 @@
       <c r="F55" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="34"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -3720,8 +3728,8 @@
       <c r="F56" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G56" s="27"/>
-      <c r="H56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="34"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -3757,8 +3765,8 @@
       <c r="F57" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G57" s="27"/>
-      <c r="H57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="34"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3794,8 +3802,8 @@
       <c r="F58" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="H58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="34"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3829,8 +3837,8 @@
       <c r="F59" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G59" s="27"/>
-      <c r="H59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="34"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3866,8 +3874,8 @@
       <c r="F60" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G60" s="27"/>
-      <c r="H60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="34"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3903,8 +3911,8 @@
       <c r="F61" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G61" s="27"/>
-      <c r="H61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="34"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3938,8 +3946,8 @@
       <c r="F62" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G62" s="27"/>
-      <c r="H62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="34"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -3973,8 +3981,8 @@
       <c r="F63" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="27"/>
-      <c r="H63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="34"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -4008,8 +4016,8 @@
       <c r="F64" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G64" s="27"/>
-      <c r="H64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="34"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -4045,8 +4053,8 @@
       <c r="F65" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G65" s="27"/>
-      <c r="H65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="34"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -4082,8 +4090,8 @@
       <c r="F66" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G66" s="27"/>
-      <c r="H66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="34"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -4119,8 +4127,8 @@
       <c r="F67" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="27"/>
-      <c r="H67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="34"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -4154,8 +4162,8 @@
       <c r="F68" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G68" s="27"/>
-      <c r="H68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="34"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -4189,8 +4197,8 @@
       <c r="F69" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G69" s="27"/>
-      <c r="H69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="34"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
@@ -4224,8 +4232,8 @@
       <c r="F70" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G70" s="27"/>
-      <c r="H70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="34"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -4261,8 +4269,8 @@
       <c r="F71" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G71" s="27"/>
-      <c r="H71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="34"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
@@ -4296,8 +4304,8 @@
       <c r="F72" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G72" s="27"/>
-      <c r="H72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="34"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
@@ -4331,8 +4339,8 @@
       <c r="F73" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G73" s="27"/>
-      <c r="H73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="34"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
@@ -4368,8 +4376,8 @@
       <c r="F74" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G74" s="27"/>
-      <c r="H74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="34"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
@@ -4403,8 +4411,8 @@
       <c r="F75" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G75" s="27"/>
-      <c r="H75" s="23"/>
+      <c r="G75" s="23"/>
+      <c r="H75" s="34"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
@@ -4438,8 +4446,8 @@
       <c r="F76" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G76" s="27"/>
-      <c r="H76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="34"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -4473,8 +4481,8 @@
       <c r="F77" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G77" s="27"/>
-      <c r="H77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="34"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
@@ -4508,8 +4516,8 @@
       <c r="F78" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G78" s="27"/>
-      <c r="H78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="34"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
@@ -4543,8 +4551,8 @@
       <c r="F79" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G79" s="27"/>
-      <c r="H79" s="23"/>
+      <c r="G79" s="23"/>
+      <c r="H79" s="34"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -4578,8 +4586,8 @@
       <c r="F80" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G80" s="27"/>
-      <c r="H80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="34"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
@@ -4613,8 +4621,8 @@
       <c r="F81" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G81" s="27"/>
-      <c r="H81" s="23"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="34"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
@@ -4650,8 +4658,8 @@
       <c r="F82" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G82" s="27"/>
-      <c r="H82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="34"/>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -4687,8 +4695,8 @@
       <c r="F83" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G83" s="27"/>
-      <c r="H83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="34"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
@@ -4722,8 +4730,8 @@
       <c r="F84" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G84" s="27"/>
-      <c r="H84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="34"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -4757,8 +4765,8 @@
       <c r="F85" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G85" s="27"/>
-      <c r="H85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="34"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -4792,8 +4800,8 @@
       <c r="F86" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G86" s="27"/>
-      <c r="H86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="34"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -4827,8 +4835,8 @@
       <c r="F87" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G87" s="27"/>
-      <c r="H87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="34"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
@@ -4862,8 +4870,8 @@
       <c r="F88" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G88" s="27"/>
-      <c r="H88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="34"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
@@ -4897,8 +4905,8 @@
       <c r="F89" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G89" s="27"/>
-      <c r="H89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="34"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
@@ -4934,8 +4942,8 @@
       <c r="F90" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G90" s="27"/>
-      <c r="H90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="34"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
@@ -4971,8 +4979,8 @@
       <c r="F91" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G91" s="27"/>
-      <c r="H91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="34"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -5008,8 +5016,8 @@
       <c r="F92" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G92" s="27"/>
-      <c r="H92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="34"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -5045,8 +5053,8 @@
       <c r="F93" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G93" s="27"/>
-      <c r="H93" s="23"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="34"/>
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
@@ -5082,8 +5090,8 @@
       <c r="F94" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G94" s="27"/>
-      <c r="H94" s="23"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="34"/>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
@@ -5119,8 +5127,8 @@
       <c r="F95" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G95" s="27"/>
-      <c r="H95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="34"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
@@ -5156,8 +5164,8 @@
       <c r="F96" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G96" s="27"/>
-      <c r="H96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="34"/>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
@@ -5193,8 +5201,8 @@
       <c r="F97" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G97" s="27"/>
-      <c r="H97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="34"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
@@ -5228,8 +5236,8 @@
       <c r="F98" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G98" s="27"/>
-      <c r="H98" s="23"/>
+      <c r="G98" s="23"/>
+      <c r="H98" s="34"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
@@ -5263,8 +5271,8 @@
       <c r="F99" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G99" s="27"/>
-      <c r="H99" s="23"/>
+      <c r="G99" s="23"/>
+      <c r="H99" s="34"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
@@ -5298,8 +5306,8 @@
       <c r="F100" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G100" s="27"/>
-      <c r="H100" s="23"/>
+      <c r="G100" s="23"/>
+      <c r="H100" s="34"/>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
@@ -5333,8 +5341,8 @@
       <c r="F101" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G101" s="27"/>
-      <c r="H101" s="23"/>
+      <c r="G101" s="23"/>
+      <c r="H101" s="34"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
@@ -5370,8 +5378,8 @@
       <c r="F102" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G102" s="27"/>
-      <c r="H102" s="23"/>
+      <c r="G102" s="23"/>
+      <c r="H102" s="34"/>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
@@ -5407,8 +5415,8 @@
       <c r="F103" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G103" s="27"/>
-      <c r="H103" s="23"/>
+      <c r="G103" s="23"/>
+      <c r="H103" s="34"/>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
@@ -5442,8 +5450,8 @@
       <c r="F104" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G104" s="27"/>
-      <c r="H104" s="23"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="34"/>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
@@ -5479,8 +5487,8 @@
       <c r="F105" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G105" s="27"/>
-      <c r="H105" s="23"/>
+      <c r="G105" s="23"/>
+      <c r="H105" s="34"/>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
@@ -5516,8 +5524,8 @@
       <c r="F106" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G106" s="27"/>
-      <c r="H106" s="23"/>
+      <c r="G106" s="23"/>
+      <c r="H106" s="34"/>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
@@ -5553,8 +5561,8 @@
       <c r="F107" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G107" s="27"/>
-      <c r="H107" s="23"/>
+      <c r="G107" s="23"/>
+      <c r="H107" s="34"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
@@ -5588,8 +5596,8 @@
       <c r="F108" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G108" s="27"/>
-      <c r="H108" s="23"/>
+      <c r="G108" s="23"/>
+      <c r="H108" s="34"/>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
@@ -5625,8 +5633,8 @@
       <c r="F109" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G109" s="27"/>
-      <c r="H109" s="23"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="34"/>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
@@ -5662,8 +5670,8 @@
       <c r="F110" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G110" s="27"/>
-      <c r="H110" s="23"/>
+      <c r="G110" s="23"/>
+      <c r="H110" s="34"/>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
@@ -5699,8 +5707,8 @@
       <c r="F111" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G111" s="28"/>
-      <c r="H111" s="23"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="34"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
@@ -5736,8 +5744,8 @@
       <c r="F112" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G112" s="27"/>
-      <c r="H112" s="24"/>
+      <c r="G112" s="23"/>
+      <c r="H112" s="36"/>
       <c r="I112" s="14"/>
       <c r="J112" s="14"/>
       <c r="K112" s="14"/>
@@ -5776,8 +5784,8 @@
       <c r="F113" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G113" s="27"/>
-      <c r="H113" s="23"/>
+      <c r="G113" s="23"/>
+      <c r="H113" s="34"/>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
@@ -5813,8 +5821,8 @@
       <c r="F114" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G114" s="27"/>
-      <c r="H114" s="23"/>
+      <c r="G114" s="23"/>
+      <c r="H114" s="34"/>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
@@ -5850,8 +5858,8 @@
       <c r="F115" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G115" s="27"/>
-      <c r="H115" s="23"/>
+      <c r="G115" s="23"/>
+      <c r="H115" s="34"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
@@ -5887,8 +5895,8 @@
       <c r="F116" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G116" s="27"/>
-      <c r="H116" s="23"/>
+      <c r="G116" s="23"/>
+      <c r="H116" s="34"/>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
@@ -5922,8 +5930,8 @@
       <c r="F117" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G117" s="27"/>
-      <c r="H117" s="23"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="34"/>
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
@@ -5959,8 +5967,8 @@
       <c r="F118" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G118" s="27"/>
-      <c r="H118" s="23"/>
+      <c r="G118" s="23"/>
+      <c r="H118" s="34"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
@@ -5996,8 +6004,8 @@
       <c r="F119" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G119" s="27"/>
-      <c r="H119" s="23"/>
+      <c r="G119" s="23"/>
+      <c r="H119" s="34"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
@@ -6031,8 +6039,8 @@
       <c r="F120" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G120" s="27"/>
-      <c r="H120" s="23"/>
+      <c r="G120" s="23"/>
+      <c r="H120" s="34"/>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
@@ -6068,8 +6076,8 @@
       <c r="F121" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G121" s="27"/>
-      <c r="H121" s="23"/>
+      <c r="G121" s="23"/>
+      <c r="H121" s="34"/>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
@@ -6105,8 +6113,8 @@
       <c r="F122" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G122" s="27"/>
-      <c r="H122" s="23"/>
+      <c r="G122" s="23"/>
+      <c r="H122" s="34"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
@@ -6142,8 +6150,8 @@
       <c r="F123" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G123" s="27"/>
-      <c r="H123" s="23"/>
+      <c r="G123" s="23"/>
+      <c r="H123" s="34"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
@@ -6179,8 +6187,8 @@
       <c r="F124" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G124" s="27"/>
-      <c r="H124" s="23"/>
+      <c r="G124" s="23"/>
+      <c r="H124" s="34"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
@@ -6216,8 +6224,8 @@
       <c r="F125" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G125" s="27"/>
-      <c r="H125" s="23"/>
+      <c r="G125" s="23"/>
+      <c r="H125" s="34"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
@@ -6253,8 +6261,8 @@
       <c r="F126" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G126" s="27"/>
-      <c r="H126" s="23"/>
+      <c r="G126" s="23"/>
+      <c r="H126" s="34"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
@@ -6290,8 +6298,8 @@
       <c r="F127" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G127" s="27"/>
-      <c r="H127" s="23"/>
+      <c r="G127" s="23"/>
+      <c r="H127" s="34"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
@@ -6327,8 +6335,8 @@
       <c r="F128" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G128" s="27"/>
-      <c r="H128" s="23"/>
+      <c r="G128" s="23"/>
+      <c r="H128" s="34"/>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
@@ -6364,8 +6372,8 @@
       <c r="F129" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G129" s="27"/>
-      <c r="H129" s="23"/>
+      <c r="G129" s="23"/>
+      <c r="H129" s="34"/>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
@@ -6401,8 +6409,8 @@
       <c r="F130" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G130" s="27"/>
-      <c r="H130" s="23"/>
+      <c r="G130" s="23"/>
+      <c r="H130" s="34"/>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3"/>
@@ -6438,8 +6446,8 @@
       <c r="F131" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G131" s="27"/>
-      <c r="H131" s="23"/>
+      <c r="G131" s="23"/>
+      <c r="H131" s="34"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
@@ -6475,8 +6483,8 @@
       <c r="F132" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G132" s="27"/>
-      <c r="H132" s="23"/>
+      <c r="G132" s="23"/>
+      <c r="H132" s="34"/>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
@@ -6512,8 +6520,8 @@
       <c r="F133" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G133" s="27"/>
-      <c r="H133" s="23"/>
+      <c r="G133" s="23"/>
+      <c r="H133" s="34"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
@@ -6549,8 +6557,8 @@
       <c r="F134" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G134" s="27"/>
-      <c r="H134" s="23"/>
+      <c r="G134" s="23"/>
+      <c r="H134" s="34"/>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
@@ -6586,8 +6594,8 @@
       <c r="F135" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G135" s="27"/>
-      <c r="H135" s="23"/>
+      <c r="G135" s="23"/>
+      <c r="H135" s="34"/>
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
@@ -6623,8 +6631,8 @@
       <c r="F136" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G136" s="27"/>
-      <c r="H136" s="23"/>
+      <c r="G136" s="23"/>
+      <c r="H136" s="34"/>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
@@ -6660,8 +6668,8 @@
       <c r="F137" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G137" s="27"/>
-      <c r="H137" s="23"/>
+      <c r="G137" s="23"/>
+      <c r="H137" s="34"/>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
@@ -6697,8 +6705,8 @@
       <c r="F138" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G138" s="27"/>
-      <c r="H138" s="23"/>
+      <c r="G138" s="23"/>
+      <c r="H138" s="34"/>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
@@ -6734,8 +6742,8 @@
       <c r="F139" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G139" s="27"/>
-      <c r="H139" s="23"/>
+      <c r="G139" s="23"/>
+      <c r="H139" s="34"/>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
@@ -6771,8 +6779,8 @@
       <c r="F140" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G140" s="27"/>
-      <c r="H140" s="23"/>
+      <c r="G140" s="23"/>
+      <c r="H140" s="34"/>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
       <c r="K140" s="3"/>
@@ -6808,8 +6816,8 @@
       <c r="F141" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G141" s="27"/>
-      <c r="H141" s="23"/>
+      <c r="G141" s="23"/>
+      <c r="H141" s="34"/>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
@@ -6845,8 +6853,8 @@
       <c r="F142" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G142" s="27"/>
-      <c r="H142" s="23"/>
+      <c r="G142" s="23"/>
+      <c r="H142" s="34"/>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
@@ -6882,8 +6890,8 @@
       <c r="F143" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G143" s="27"/>
-      <c r="H143" s="23"/>
+      <c r="G143" s="23"/>
+      <c r="H143" s="34"/>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
       <c r="K143" s="3"/>
@@ -6919,8 +6927,8 @@
       <c r="F144" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G144" s="27"/>
-      <c r="H144" s="23"/>
+      <c r="G144" s="23"/>
+      <c r="H144" s="34"/>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
@@ -6956,8 +6964,8 @@
       <c r="F145" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G145" s="27"/>
-      <c r="H145" s="23"/>
+      <c r="G145" s="23"/>
+      <c r="H145" s="34"/>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
@@ -6993,8 +7001,8 @@
       <c r="F146" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G146" s="27"/>
-      <c r="H146" s="23"/>
+      <c r="G146" s="23"/>
+      <c r="H146" s="34"/>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
@@ -7028,8 +7036,8 @@
       <c r="F147" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G147" s="27"/>
-      <c r="H147" s="23"/>
+      <c r="G147" s="23"/>
+      <c r="H147" s="34"/>
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
@@ -7065,8 +7073,8 @@
       <c r="F148" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G148" s="27"/>
-      <c r="H148" s="23"/>
+      <c r="G148" s="23"/>
+      <c r="H148" s="34"/>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
@@ -7102,8 +7110,8 @@
       <c r="F149" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G149" s="27"/>
-      <c r="H149" s="23"/>
+      <c r="G149" s="23"/>
+      <c r="H149" s="34"/>
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
       <c r="K149" s="3"/>
@@ -7139,8 +7147,8 @@
       <c r="F150" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G150" s="27"/>
-      <c r="H150" s="23"/>
+      <c r="G150" s="23"/>
+      <c r="H150" s="34"/>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
@@ -7176,8 +7184,8 @@
       <c r="F151" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G151" s="27"/>
-      <c r="H151" s="23"/>
+      <c r="G151" s="23"/>
+      <c r="H151" s="34"/>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
@@ -7213,8 +7221,8 @@
       <c r="F152" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G152" s="27"/>
-      <c r="H152" s="23"/>
+      <c r="G152" s="23"/>
+      <c r="H152" s="34"/>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
       <c r="K152" s="3"/>
@@ -7248,8 +7256,8 @@
       <c r="F153" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G153" s="27"/>
-      <c r="H153" s="23"/>
+      <c r="G153" s="23"/>
+      <c r="H153" s="34"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
@@ -7283,8 +7291,8 @@
       <c r="F154" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G154" s="27"/>
-      <c r="H154" s="23"/>
+      <c r="G154" s="23"/>
+      <c r="H154" s="34"/>
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
@@ -7320,8 +7328,8 @@
       <c r="F155" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G155" s="27"/>
-      <c r="H155" s="23"/>
+      <c r="G155" s="23"/>
+      <c r="H155" s="34"/>
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
@@ -7357,8 +7365,8 @@
       <c r="F156" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G156" s="27"/>
-      <c r="H156" s="23"/>
+      <c r="G156" s="23"/>
+      <c r="H156" s="34"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
@@ -7392,8 +7400,8 @@
       <c r="F157" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G157" s="27"/>
-      <c r="H157" s="23"/>
+      <c r="G157" s="23"/>
+      <c r="H157" s="34"/>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
@@ -7429,8 +7437,8 @@
       <c r="F158" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G158" s="27"/>
-      <c r="H158" s="23"/>
+      <c r="G158" s="23"/>
+      <c r="H158" s="34"/>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
@@ -7466,8 +7474,8 @@
       <c r="F159" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G159" s="27"/>
-      <c r="H159" s="23"/>
+      <c r="G159" s="23"/>
+      <c r="H159" s="34"/>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
@@ -7503,8 +7511,8 @@
       <c r="F160" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G160" s="27"/>
-      <c r="H160" s="23"/>
+      <c r="G160" s="23"/>
+      <c r="H160" s="34"/>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
@@ -7540,8 +7548,8 @@
       <c r="F161" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G161" s="27"/>
-      <c r="H161" s="23"/>
+      <c r="G161" s="23"/>
+      <c r="H161" s="34"/>
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
@@ -7575,8 +7583,8 @@
       <c r="F162" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G162" s="27"/>
-      <c r="H162" s="23"/>
+      <c r="G162" s="23"/>
+      <c r="H162" s="34"/>
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
       <c r="K162" s="3"/>
@@ -7612,8 +7620,8 @@
       <c r="F163" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G163" s="27"/>
-      <c r="H163" s="23"/>
+      <c r="G163" s="23"/>
+      <c r="H163" s="34"/>
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
@@ -7649,8 +7657,8 @@
       <c r="F164" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G164" s="27"/>
-      <c r="H164" s="23"/>
+      <c r="G164" s="23"/>
+      <c r="H164" s="34"/>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
@@ -7684,8 +7692,8 @@
       <c r="F165" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G165" s="27"/>
-      <c r="H165" s="23"/>
+      <c r="G165" s="23"/>
+      <c r="H165" s="34"/>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
       <c r="K165" s="3"/>
@@ -7719,8 +7727,8 @@
       <c r="F166" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G166" s="27"/>
-      <c r="H166" s="23"/>
+      <c r="G166" s="23"/>
+      <c r="H166" s="34"/>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
@@ -7756,8 +7764,8 @@
       <c r="F167" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G167" s="27"/>
-      <c r="H167" s="23"/>
+      <c r="G167" s="23"/>
+      <c r="H167" s="34"/>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
@@ -7791,8 +7799,8 @@
       <c r="F168" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="G168" s="27"/>
-      <c r="H168" s="23"/>
+      <c r="G168" s="23"/>
+      <c r="H168" s="34"/>
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
@@ -7826,8 +7834,8 @@
       <c r="F169" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="G169" s="27"/>
-      <c r="H169" s="23"/>
+      <c r="G169" s="23"/>
+      <c r="H169" s="34"/>
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
@@ -7861,8 +7869,8 @@
       <c r="F170" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G170" s="27"/>
-      <c r="H170" s="23"/>
+      <c r="G170" s="23"/>
+      <c r="H170" s="34"/>
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
       <c r="K170" s="3"/>
@@ -7898,8 +7906,8 @@
       <c r="F171" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G171" s="27"/>
-      <c r="H171" s="23"/>
+      <c r="G171" s="23"/>
+      <c r="H171" s="34"/>
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
@@ -7935,8 +7943,8 @@
       <c r="F172" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G172" s="27"/>
-      <c r="H172" s="23"/>
+      <c r="G172" s="23"/>
+      <c r="H172" s="34"/>
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
@@ -7972,8 +7980,8 @@
       <c r="F173" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G173" s="27"/>
-      <c r="H173" s="23"/>
+      <c r="G173" s="23"/>
+      <c r="H173" s="34"/>
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
@@ -8009,8 +8017,8 @@
       <c r="F174" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G174" s="27"/>
-      <c r="H174" s="23"/>
+      <c r="G174" s="23"/>
+      <c r="H174" s="34"/>
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
       <c r="K174" s="3"/>
@@ -8044,8 +8052,8 @@
       <c r="F175" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G175" s="27"/>
-      <c r="H175" s="23"/>
+      <c r="G175" s="23"/>
+      <c r="H175" s="34"/>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
@@ -8079,8 +8087,8 @@
       <c r="F176" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G176" s="27"/>
-      <c r="H176" s="23"/>
+      <c r="G176" s="23"/>
+      <c r="H176" s="34"/>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
       <c r="K176" s="3"/>
@@ -8114,8 +8122,8 @@
       <c r="F177" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G177" s="27"/>
-      <c r="H177" s="23"/>
+      <c r="G177" s="23"/>
+      <c r="H177" s="34"/>
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
       <c r="K177" s="3"/>
@@ -8149,8 +8157,8 @@
       <c r="F178" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G178" s="27"/>
-      <c r="H178" s="23"/>
+      <c r="G178" s="23"/>
+      <c r="H178" s="34"/>
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
       <c r="K178" s="3"/>
@@ -8184,8 +8192,8 @@
       <c r="F179" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G179" s="27"/>
-      <c r="H179" s="23"/>
+      <c r="G179" s="23"/>
+      <c r="H179" s="34"/>
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
       <c r="K179" s="3"/>
@@ -8219,8 +8227,8 @@
       <c r="F180" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G180" s="27"/>
-      <c r="H180" s="23"/>
+      <c r="G180" s="23"/>
+      <c r="H180" s="34"/>
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
       <c r="K180" s="3"/>
@@ -8254,8 +8262,8 @@
       <c r="F181" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G181" s="27"/>
-      <c r="H181" s="23"/>
+      <c r="G181" s="23"/>
+      <c r="H181" s="34"/>
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
       <c r="K181" s="3"/>
@@ -8289,8 +8297,8 @@
       <c r="F182" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G182" s="27"/>
-      <c r="H182" s="23"/>
+      <c r="G182" s="23"/>
+      <c r="H182" s="34"/>
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
       <c r="K182" s="3"/>
@@ -8324,8 +8332,8 @@
       <c r="F183" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G183" s="27"/>
-      <c r="H183" s="23"/>
+      <c r="G183" s="23"/>
+      <c r="H183" s="34"/>
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
       <c r="K183" s="3"/>
@@ -8361,8 +8369,8 @@
       <c r="F184" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G184" s="27"/>
-      <c r="H184" s="23"/>
+      <c r="G184" s="23"/>
+      <c r="H184" s="34"/>
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
       <c r="K184" s="3"/>
@@ -8398,8 +8406,8 @@
       <c r="F185" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G185" s="27"/>
-      <c r="H185" s="23"/>
+      <c r="G185" s="23"/>
+      <c r="H185" s="34"/>
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
       <c r="K185" s="3"/>
@@ -8435,8 +8443,8 @@
       <c r="F186" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G186" s="27"/>
-      <c r="H186" s="23"/>
+      <c r="G186" s="23"/>
+      <c r="H186" s="34"/>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
       <c r="K186" s="3"/>
@@ -8472,8 +8480,8 @@
       <c r="F187" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G187" s="27"/>
-      <c r="H187" s="23"/>
+      <c r="G187" s="23"/>
+      <c r="H187" s="34"/>
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
       <c r="K187" s="3"/>
@@ -8509,8 +8517,8 @@
       <c r="F188" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G188" s="27"/>
-      <c r="H188" s="23"/>
+      <c r="G188" s="23"/>
+      <c r="H188" s="34"/>
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
       <c r="K188" s="3"/>
@@ -8546,8 +8554,8 @@
       <c r="F189" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G189" s="27"/>
-      <c r="H189" s="23"/>
+      <c r="G189" s="23"/>
+      <c r="H189" s="34"/>
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
       <c r="K189" s="3"/>
@@ -8583,8 +8591,8 @@
       <c r="F190" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G190" s="27"/>
-      <c r="H190" s="23"/>
+      <c r="G190" s="23"/>
+      <c r="H190" s="34"/>
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
       <c r="K190" s="3"/>
@@ -8620,8 +8628,8 @@
       <c r="F191" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G191" s="27"/>
-      <c r="H191" s="23"/>
+      <c r="G191" s="23"/>
+      <c r="H191" s="34"/>
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
       <c r="K191" s="3"/>
@@ -8657,8 +8665,8 @@
       <c r="F192" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G192" s="27"/>
-      <c r="H192" s="23"/>
+      <c r="G192" s="23"/>
+      <c r="H192" s="34"/>
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
       <c r="K192" s="3"/>
@@ -8694,8 +8702,8 @@
       <c r="F193" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G193" s="27"/>
-      <c r="H193" s="23"/>
+      <c r="G193" s="23"/>
+      <c r="H193" s="34"/>
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
       <c r="K193" s="3"/>
@@ -8731,8 +8739,8 @@
       <c r="F194" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G194" s="27"/>
-      <c r="H194" s="23"/>
+      <c r="G194" s="23"/>
+      <c r="H194" s="34"/>
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
       <c r="K194" s="3"/>
@@ -8768,8 +8776,8 @@
       <c r="F195" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G195" s="27"/>
-      <c r="H195" s="23"/>
+      <c r="G195" s="23"/>
+      <c r="H195" s="34"/>
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
       <c r="K195" s="3"/>
@@ -8805,8 +8813,8 @@
       <c r="F196" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G196" s="27"/>
-      <c r="H196" s="23"/>
+      <c r="G196" s="23"/>
+      <c r="H196" s="34"/>
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
       <c r="K196" s="3"/>
@@ -8842,8 +8850,8 @@
       <c r="F197" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G197" s="27"/>
-      <c r="H197" s="23"/>
+      <c r="G197" s="23"/>
+      <c r="H197" s="34"/>
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
       <c r="K197" s="3"/>
@@ -8879,8 +8887,8 @@
       <c r="F198" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G198" s="27"/>
-      <c r="H198" s="23"/>
+      <c r="G198" s="23"/>
+      <c r="H198" s="34"/>
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
       <c r="K198" s="3"/>
@@ -8916,8 +8924,8 @@
       <c r="F199" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G199" s="27"/>
-      <c r="H199" s="23"/>
+      <c r="G199" s="23"/>
+      <c r="H199" s="34"/>
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
       <c r="K199" s="3"/>
@@ -8951,8 +8959,8 @@
       <c r="F200" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G200" s="27"/>
-      <c r="H200" s="23"/>
+      <c r="G200" s="23"/>
+      <c r="H200" s="34"/>
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
       <c r="K200" s="3"/>
@@ -8988,8 +8996,8 @@
       <c r="F201" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G201" s="27"/>
-      <c r="H201" s="23"/>
+      <c r="G201" s="23"/>
+      <c r="H201" s="34"/>
       <c r="I201" s="3"/>
       <c r="J201" s="3"/>
       <c r="K201" s="3"/>
@@ -9025,8 +9033,8 @@
       <c r="F202" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G202" s="27"/>
-      <c r="H202" s="23"/>
+      <c r="G202" s="23"/>
+      <c r="H202" s="34"/>
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
       <c r="K202" s="3"/>
@@ -9060,8 +9068,8 @@
       <c r="F203" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G203" s="27"/>
-      <c r="H203" s="23"/>
+      <c r="G203" s="23"/>
+      <c r="H203" s="34"/>
       <c r="I203" s="3"/>
       <c r="J203" s="3"/>
       <c r="K203" s="3"/>
@@ -9095,8 +9103,8 @@
       <c r="F204" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G204" s="27"/>
-      <c r="H204" s="23"/>
+      <c r="G204" s="23"/>
+      <c r="H204" s="34"/>
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
       <c r="K204" s="3"/>
@@ -9130,8 +9138,8 @@
       <c r="F205" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G205" s="27"/>
-      <c r="H205" s="23"/>
+      <c r="G205" s="23"/>
+      <c r="H205" s="34"/>
       <c r="I205" s="3"/>
       <c r="J205" s="3"/>
       <c r="K205" s="3"/>
@@ -9165,8 +9173,8 @@
       <c r="F206" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G206" s="27"/>
-      <c r="H206" s="23"/>
+      <c r="G206" s="23"/>
+      <c r="H206" s="34"/>
       <c r="I206" s="3"/>
       <c r="J206" s="3"/>
       <c r="K206" s="3"/>
@@ -9200,8 +9208,8 @@
       <c r="F207" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G207" s="27"/>
-      <c r="H207" s="23"/>
+      <c r="G207" s="23"/>
+      <c r="H207" s="34"/>
       <c r="I207" s="3"/>
       <c r="J207" s="3"/>
       <c r="K207" s="3"/>
@@ -9235,8 +9243,8 @@
       <c r="F208" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G208" s="27"/>
-      <c r="H208" s="23"/>
+      <c r="G208" s="23"/>
+      <c r="H208" s="34"/>
       <c r="I208" s="3"/>
       <c r="J208" s="3"/>
       <c r="K208" s="3"/>
@@ -9272,8 +9280,8 @@
       <c r="F209" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G209" s="27"/>
-      <c r="H209" s="23"/>
+      <c r="G209" s="23"/>
+      <c r="H209" s="34"/>
       <c r="I209" s="3"/>
       <c r="J209" s="3"/>
       <c r="K209" s="3"/>
@@ -9307,8 +9315,8 @@
       <c r="F210" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G210" s="27"/>
-      <c r="H210" s="23"/>
+      <c r="G210" s="23"/>
+      <c r="H210" s="34"/>
       <c r="I210" s="3"/>
       <c r="J210" s="3"/>
       <c r="K210" s="3"/>
@@ -9342,8 +9350,8 @@
       <c r="F211" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G211" s="27"/>
-      <c r="H211" s="23"/>
+      <c r="G211" s="23"/>
+      <c r="H211" s="34"/>
       <c r="I211" s="3"/>
       <c r="J211" s="3"/>
       <c r="K211" s="3"/>
@@ -9377,8 +9385,8 @@
       <c r="F212" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G212" s="27"/>
-      <c r="H212" s="23"/>
+      <c r="G212" s="23"/>
+      <c r="H212" s="34"/>
       <c r="I212" s="3"/>
       <c r="J212" s="3"/>
       <c r="K212" s="3"/>
@@ -9412,8 +9420,8 @@
       <c r="F213" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G213" s="27"/>
-      <c r="H213" s="23"/>
+      <c r="G213" s="23"/>
+      <c r="H213" s="34"/>
       <c r="I213" s="3"/>
       <c r="J213" s="3"/>
       <c r="K213" s="3"/>
@@ -9447,8 +9455,8 @@
       <c r="F214" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G214" s="27"/>
-      <c r="H214" s="23"/>
+      <c r="G214" s="23"/>
+      <c r="H214" s="34"/>
       <c r="I214" s="3"/>
       <c r="J214" s="3"/>
       <c r="K214" s="3"/>
@@ -9484,8 +9492,8 @@
       <c r="F215" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G215" s="27"/>
-      <c r="H215" s="23"/>
+      <c r="G215" s="23"/>
+      <c r="H215" s="34"/>
       <c r="I215" s="3"/>
       <c r="J215" s="3"/>
       <c r="K215" s="3"/>
@@ -9519,8 +9527,8 @@
       <c r="F216" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G216" s="27"/>
-      <c r="H216" s="23"/>
+      <c r="G216" s="23"/>
+      <c r="H216" s="34"/>
       <c r="I216" s="3"/>
       <c r="J216" s="3"/>
       <c r="K216" s="3"/>
@@ -9554,8 +9562,8 @@
       <c r="F217" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G217" s="27"/>
-      <c r="H217" s="23"/>
+      <c r="G217" s="23"/>
+      <c r="H217" s="34"/>
       <c r="I217" s="3"/>
       <c r="J217" s="3"/>
       <c r="K217" s="3"/>
@@ -9591,8 +9599,8 @@
       <c r="F218" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G218" s="27"/>
-      <c r="H218" s="23"/>
+      <c r="G218" s="23"/>
+      <c r="H218" s="34"/>
       <c r="I218" s="3"/>
       <c r="J218" s="3"/>
       <c r="K218" s="3"/>
@@ -9626,8 +9634,8 @@
       <c r="F219" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G219" s="27"/>
-      <c r="H219" s="23"/>
+      <c r="G219" s="23"/>
+      <c r="H219" s="34"/>
       <c r="I219" s="3"/>
       <c r="J219" s="3"/>
       <c r="K219" s="3"/>
@@ -9661,8 +9669,8 @@
       <c r="F220" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G220" s="27"/>
-      <c r="H220" s="23"/>
+      <c r="G220" s="23"/>
+      <c r="H220" s="34"/>
       <c r="I220" s="3"/>
       <c r="J220" s="3"/>
       <c r="K220" s="3"/>
@@ -9696,8 +9704,8 @@
       <c r="F221" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G221" s="27"/>
-      <c r="H221" s="23"/>
+      <c r="G221" s="23"/>
+      <c r="H221" s="34"/>
       <c r="I221" s="3"/>
       <c r="J221" s="3"/>
       <c r="K221" s="3"/>
@@ -9731,8 +9739,8 @@
       <c r="F222" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G222" s="27"/>
-      <c r="H222" s="23"/>
+      <c r="G222" s="23"/>
+      <c r="H222" s="34"/>
       <c r="I222" s="3"/>
       <c r="J222" s="3"/>
       <c r="K222" s="3"/>
@@ -9766,8 +9774,8 @@
       <c r="F223" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G223" s="27"/>
-      <c r="H223" s="23"/>
+      <c r="G223" s="23"/>
+      <c r="H223" s="34"/>
       <c r="I223" s="3"/>
       <c r="J223" s="3"/>
       <c r="K223" s="3"/>
@@ -9801,8 +9809,8 @@
       <c r="F224" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G224" s="27"/>
-      <c r="H224" s="23"/>
+      <c r="G224" s="23"/>
+      <c r="H224" s="34"/>
       <c r="I224" s="3"/>
       <c r="J224" s="3"/>
       <c r="K224" s="3"/>
@@ -9836,8 +9844,8 @@
       <c r="F225" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G225" s="27"/>
-      <c r="H225" s="23"/>
+      <c r="G225" s="23"/>
+      <c r="H225" s="34"/>
       <c r="I225" s="3"/>
       <c r="J225" s="3"/>
       <c r="K225" s="3"/>
@@ -9871,8 +9879,8 @@
       <c r="F226" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G226" s="27"/>
-      <c r="H226" s="23"/>
+      <c r="G226" s="23"/>
+      <c r="H226" s="34"/>
       <c r="I226" s="3"/>
       <c r="J226" s="3"/>
       <c r="K226" s="3"/>
@@ -9908,8 +9916,8 @@
       <c r="F227" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G227" s="27"/>
-      <c r="H227" s="23"/>
+      <c r="G227" s="23"/>
+      <c r="H227" s="34"/>
       <c r="I227" s="3"/>
       <c r="J227" s="3"/>
       <c r="K227" s="3"/>
@@ -9943,8 +9951,8 @@
       <c r="F228" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G228" s="27"/>
-      <c r="H228" s="23"/>
+      <c r="G228" s="23"/>
+      <c r="H228" s="34"/>
       <c r="I228" s="3"/>
       <c r="J228" s="3"/>
       <c r="K228" s="3"/>
@@ -9980,8 +9988,8 @@
       <c r="F229" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G229" s="27"/>
-      <c r="H229" s="23"/>
+      <c r="G229" s="23"/>
+      <c r="H229" s="34"/>
       <c r="I229" s="3"/>
       <c r="J229" s="3"/>
       <c r="K229" s="3"/>
@@ -10017,8 +10025,8 @@
       <c r="F230" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G230" s="27"/>
-      <c r="H230" s="23"/>
+      <c r="G230" s="23"/>
+      <c r="H230" s="34"/>
       <c r="I230" s="3"/>
       <c r="J230" s="3"/>
       <c r="K230" s="3"/>
@@ -10052,8 +10060,8 @@
       <c r="F231" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G231" s="27"/>
-      <c r="H231" s="23"/>
+      <c r="G231" s="23"/>
+      <c r="H231" s="34"/>
       <c r="I231" s="3"/>
       <c r="J231" s="3"/>
       <c r="K231" s="3"/>
@@ -10087,8 +10095,8 @@
       <c r="F232" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G232" s="27"/>
-      <c r="H232" s="23"/>
+      <c r="G232" s="23"/>
+      <c r="H232" s="34"/>
       <c r="I232" s="3"/>
       <c r="J232" s="3"/>
       <c r="K232" s="3"/>
@@ -10122,8 +10130,8 @@
       <c r="F233" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G233" s="27"/>
-      <c r="H233" s="23"/>
+      <c r="G233" s="23"/>
+      <c r="H233" s="34"/>
       <c r="I233" s="3"/>
       <c r="J233" s="3"/>
       <c r="K233" s="3"/>
@@ -10159,8 +10167,8 @@
       <c r="F234" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G234" s="27"/>
-      <c r="H234" s="23"/>
+      <c r="G234" s="23"/>
+      <c r="H234" s="34"/>
       <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
@@ -10196,8 +10204,8 @@
       <c r="F235" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G235" s="27"/>
-      <c r="H235" s="23"/>
+      <c r="G235" s="23"/>
+      <c r="H235" s="34"/>
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
       <c r="K235" s="3"/>
@@ -10231,8 +10239,8 @@
       <c r="F236" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G236" s="27"/>
-      <c r="H236" s="23"/>
+      <c r="G236" s="23"/>
+      <c r="H236" s="34"/>
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
@@ -10266,8 +10274,8 @@
       <c r="F237" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G237" s="27"/>
-      <c r="H237" s="23"/>
+      <c r="G237" s="23"/>
+      <c r="H237" s="34"/>
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="3"/>
@@ -10303,8 +10311,8 @@
       <c r="F238" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G238" s="27"/>
-      <c r="H238" s="23"/>
+      <c r="G238" s="23"/>
+      <c r="H238" s="34"/>
       <c r="I238" s="3"/>
       <c r="J238" s="3"/>
       <c r="K238" s="3"/>
@@ -10338,8 +10346,8 @@
       <c r="F239" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G239" s="27"/>
-      <c r="H239" s="23"/>
+      <c r="G239" s="23"/>
+      <c r="H239" s="34"/>
       <c r="I239" s="3"/>
       <c r="J239" s="3"/>
       <c r="K239" s="3"/>
@@ -10373,8 +10381,8 @@
       <c r="F240" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G240" s="27"/>
-      <c r="H240" s="23"/>
+      <c r="G240" s="23"/>
+      <c r="H240" s="34"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3"/>
       <c r="K240" s="3"/>
@@ -10410,8 +10418,8 @@
       <c r="F241" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G241" s="27"/>
-      <c r="H241" s="23"/>
+      <c r="G241" s="23"/>
+      <c r="H241" s="34"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
       <c r="K241" s="3"/>
@@ -10447,8 +10455,8 @@
       <c r="F242" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G242" s="27"/>
-      <c r="H242" s="23"/>
+      <c r="G242" s="23"/>
+      <c r="H242" s="34"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3"/>
       <c r="K242" s="3"/>
@@ -10484,8 +10492,8 @@
       <c r="F243" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G243" s="27"/>
-      <c r="H243" s="23"/>
+      <c r="G243" s="23"/>
+      <c r="H243" s="34"/>
       <c r="I243" s="3"/>
       <c r="J243" s="3"/>
       <c r="K243" s="3"/>
@@ -10521,8 +10529,8 @@
       <c r="F244" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G244" s="27"/>
-      <c r="H244" s="23"/>
+      <c r="G244" s="23"/>
+      <c r="H244" s="34"/>
       <c r="I244" s="3"/>
       <c r="J244" s="3"/>
       <c r="K244" s="3"/>
@@ -10558,8 +10566,8 @@
       <c r="F245" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G245" s="27"/>
-      <c r="H245" s="23"/>
+      <c r="G245" s="23"/>
+      <c r="H245" s="34"/>
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
       <c r="K245" s="3"/>
@@ -10595,8 +10603,8 @@
       <c r="F246" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G246" s="27"/>
-      <c r="H246" s="23"/>
+      <c r="G246" s="23"/>
+      <c r="H246" s="34"/>
       <c r="I246" s="3"/>
       <c r="J246" s="3"/>
       <c r="K246" s="3"/>
@@ -10632,8 +10640,8 @@
       <c r="F247" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G247" s="27"/>
-      <c r="H247" s="23"/>
+      <c r="G247" s="23"/>
+      <c r="H247" s="34"/>
       <c r="I247" s="3"/>
       <c r="J247" s="3"/>
       <c r="K247" s="3"/>
@@ -10669,8 +10677,8 @@
       <c r="F248" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G248" s="27"/>
-      <c r="H248" s="23"/>
+      <c r="G248" s="23"/>
+      <c r="H248" s="34"/>
       <c r="I248" s="3"/>
       <c r="J248" s="3"/>
       <c r="K248" s="3"/>
@@ -10706,8 +10714,8 @@
       <c r="F249" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G249" s="27"/>
-      <c r="H249" s="23"/>
+      <c r="G249" s="23"/>
+      <c r="H249" s="34"/>
       <c r="I249" s="3"/>
       <c r="J249" s="3"/>
       <c r="K249" s="3"/>
@@ -10741,8 +10749,8 @@
       <c r="F250" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G250" s="27"/>
-      <c r="H250" s="23"/>
+      <c r="G250" s="23"/>
+      <c r="H250" s="34"/>
       <c r="I250" s="3"/>
       <c r="J250" s="3"/>
       <c r="K250" s="3"/>
@@ -10776,8 +10784,8 @@
       <c r="F251" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G251" s="27"/>
-      <c r="H251" s="23"/>
+      <c r="G251" s="23"/>
+      <c r="H251" s="34"/>
       <c r="I251" s="3"/>
       <c r="J251" s="3"/>
       <c r="K251" s="3"/>
@@ -10811,8 +10819,8 @@
       <c r="F252" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G252" s="27"/>
-      <c r="H252" s="23"/>
+      <c r="G252" s="23"/>
+      <c r="H252" s="34"/>
       <c r="I252" s="3"/>
       <c r="J252" s="3"/>
       <c r="K252" s="3"/>
@@ -10846,8 +10854,8 @@
       <c r="F253" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G253" s="27"/>
-      <c r="H253" s="23"/>
+      <c r="G253" s="23"/>
+      <c r="H253" s="34"/>
       <c r="I253" s="3"/>
       <c r="J253" s="3"/>
       <c r="K253" s="3"/>
@@ -10881,8 +10889,8 @@
       <c r="F254" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G254" s="27"/>
-      <c r="H254" s="23"/>
+      <c r="G254" s="23"/>
+      <c r="H254" s="34"/>
       <c r="I254" s="3"/>
       <c r="J254" s="3"/>
       <c r="K254" s="3"/>
@@ -10916,8 +10924,8 @@
       <c r="F255" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G255" s="27"/>
-      <c r="H255" s="23"/>
+      <c r="G255" s="23"/>
+      <c r="H255" s="34"/>
       <c r="I255" s="3"/>
       <c r="J255" s="3"/>
       <c r="K255" s="3"/>
@@ -10951,8 +10959,8 @@
       <c r="F256" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G256" s="27"/>
-      <c r="H256" s="23"/>
+      <c r="G256" s="23"/>
+      <c r="H256" s="34"/>
       <c r="I256" s="3"/>
       <c r="J256" s="3"/>
       <c r="K256" s="3"/>
@@ -10986,8 +10994,8 @@
       <c r="F257" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G257" s="27"/>
-      <c r="H257" s="23"/>
+      <c r="G257" s="23"/>
+      <c r="H257" s="34"/>
       <c r="I257" s="3"/>
       <c r="J257" s="3"/>
       <c r="K257" s="3"/>
@@ -11023,8 +11031,8 @@
       <c r="F258" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G258" s="27"/>
-      <c r="H258" s="23"/>
+      <c r="G258" s="23"/>
+      <c r="H258" s="34"/>
       <c r="I258" s="3"/>
       <c r="J258" s="3"/>
       <c r="K258" s="3"/>
@@ -11058,8 +11066,8 @@
       <c r="F259" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G259" s="27"/>
-      <c r="H259" s="23"/>
+      <c r="G259" s="23"/>
+      <c r="H259" s="34"/>
       <c r="I259" s="3"/>
       <c r="J259" s="3"/>
       <c r="K259" s="3"/>
@@ -11089,8 +11097,8 @@
       <c r="F260" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G260" s="27"/>
-      <c r="H260" s="23"/>
+      <c r="G260" s="23"/>
+      <c r="H260" s="34"/>
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
       <c r="K260" s="3"/>
@@ -11120,8 +11128,8 @@
       <c r="F261" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G261" s="27"/>
-      <c r="H261" s="23"/>
+      <c r="G261" s="23"/>
+      <c r="H261" s="34"/>
       <c r="I261" s="3"/>
       <c r="J261" s="3"/>
       <c r="K261" s="3"/>
@@ -11151,8 +11159,8 @@
       <c r="F262" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G262" s="27"/>
-      <c r="H262" s="23"/>
+      <c r="G262" s="23"/>
+      <c r="H262" s="34"/>
       <c r="I262" s="3"/>
       <c r="J262" s="3"/>
       <c r="K262" s="3"/>
@@ -11182,8 +11190,8 @@
       <c r="F263" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G263" s="27"/>
-      <c r="H263" s="23"/>
+      <c r="G263" s="23"/>
+      <c r="H263" s="34"/>
       <c r="I263" s="3"/>
       <c r="J263" s="3"/>
       <c r="K263" s="3"/>
@@ -11207,8 +11215,8 @@
       <c r="D264" s="5"/>
       <c r="E264" s="5"/>
       <c r="F264" s="5"/>
-      <c r="G264" s="27"/>
-      <c r="H264" s="23"/>
+      <c r="G264" s="23"/>
+      <c r="H264" s="34"/>
       <c r="I264" s="3"/>
       <c r="J264" s="3"/>
       <c r="K264" s="3"/>
@@ -11232,8 +11240,8 @@
       <c r="D265" s="20"/>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
-      <c r="G265" s="29"/>
-      <c r="H265" s="23"/>
+      <c r="G265" s="25"/>
+      <c r="H265" s="34"/>
       <c r="I265" s="3"/>
       <c r="J265" s="3"/>
       <c r="K265" s="3"/>
@@ -11257,7 +11265,7 @@
       <c r="D266" s="20"/>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
-      <c r="G266" s="29"/>
+      <c r="G266" s="25"/>
     </row>
     <row r="267" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="20"/>
@@ -11266,7 +11274,7 @@
       <c r="D267" s="20"/>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
-      <c r="G267" s="29"/>
+      <c r="G267" s="25"/>
     </row>
     <row r="268" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="20"/>

</xml_diff>

<commit_message>
getCounts function has been added
</commit_message>
<xml_diff>
--- a/Sheets/July_Beverage_Inventory_2024_Luis.xlsx
+++ b/Sheets/July_Beverage_Inventory_2024_Luis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelangelweill/Documents/bootcamp/Hiyakawa-Inventory/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13D8D0-EC1C-364F-BB4F-632F89F65EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B2DCB3-0F5C-4443-ABE7-F2FD298E951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AA23DA77-A71A-4544-8D83-D05CD8F00C4B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{AA23DA77-A71A-4544-8D83-D05CD8F00C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="July Inventory (2)" sheetId="1" r:id="rId1"/>
@@ -1740,9 +1740,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1852,9 +1852,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="23"/>
-      <c r="H3" s="34">
-        <v>1</v>
-      </c>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1889,7 +1887,9 @@
         <v>12</v>
       </c>
       <c r="G4" s="23"/>
-      <c r="H4" s="34"/>
+      <c r="H4" s="34">
+        <v>2</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1924,7 +1924,9 @@
         <v>12</v>
       </c>
       <c r="G5" s="23"/>
-      <c r="H5" s="34"/>
+      <c r="H5" s="34">
+        <v>3</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1959,7 +1961,9 @@
         <v>12</v>
       </c>
       <c r="G6" s="23"/>
-      <c r="H6" s="34"/>
+      <c r="H6" s="34">
+        <v>4</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>

</xml_diff>